<commit_message>
fixed issue with same user with multiple classes
</commit_message>
<xml_diff>
--- a/StudentsData.xlsx
+++ b/StudentsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\474-IntelligentSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C56276-2B05-48A9-B026-E92579944F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E55E39-B982-4870-B2DB-62FBDD8968C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21615" yWindow="-14160" windowWidth="17280" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>First Name</t>
   </si>
@@ -482,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -628,6 +628,29 @@
         <v>31</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>